<commit_message>
Files must now only contain account, debit and credit column
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E26FAA18-BAC9-450D-9471-DBFBF0AEBAA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
   <si>
     <t/>
   </si>
@@ -36,36 +36,21 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Finance Expenses</t>
-  </si>
-  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
-    <t>Income Tax Expense</t>
-  </si>
-  <si>
     <t>Income tax expense</t>
   </si>
   <si>
-    <t>Administrative Expenses</t>
-  </si>
-  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
-    <t>Other Income</t>
-  </si>
-  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
-    <t>Distribution and Marketing Expenses</t>
-  </si>
-  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -135,51 +120,30 @@
     <t>Accounting fee</t>
   </si>
   <si>
-    <t>Cost of Sales</t>
-  </si>
-  <si>
     <t>Purchases</t>
   </si>
   <si>
-    <t>Revenue</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>Retained Profits</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
-    <t>Share Capital</t>
-  </si>
-  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
-    <t>Current Income Tax Liabilities</t>
-  </si>
-  <si>
     <t>Income tax payable</t>
   </si>
   <si>
-    <t>Amount owing from a Shareholder</t>
-  </si>
-  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
-    <t>GST Payables</t>
-  </si>
-  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -201,15 +165,9 @@
     <t>Prepayments</t>
   </si>
   <si>
-    <t>Deposits</t>
-  </si>
-  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
-    <t>Plant and Equipment</t>
-  </si>
-  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -237,9 +195,6 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
-    <t>Bank Balances</t>
-  </si>
-  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -259,15 +214,6 @@
   </si>
   <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>December 2016</t>
-  </si>
-  <si>
-    <t>Trial Balance</t>
-  </si>
-  <si>
-    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -988,7 +934,7 @@
   <dimension ref="A1:AA81"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1399,9 +1345,7 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63" t="s">
-        <v>79</v>
-      </c>
+      <c r="E2" s="63"/>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1411,9 +1355,7 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="59"/>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1423,9 +1365,7 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E4" s="59"/>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1435,9 +1375,7 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E5" s="59"/>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1447,9 +1385,7 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="59"/>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1459,9 +1395,7 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56" t="s">
-        <v>78</v>
-      </c>
+      <c r="E7" s="56"/>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1471,9 +1405,7 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52" t="s">
-        <v>77</v>
-      </c>
+      <c r="E8" s="52"/>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1494,15 +1426,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1512,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1520,9 +1452,7 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H11" s="31"/>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1549,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1557,16 +1487,14 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1574,16 +1502,14 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1591,16 +1517,14 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1614,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1622,16 +1546,13 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
-      <c r="H16" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1639,16 +1560,13 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
-      <c r="H17" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1656,16 +1574,13 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
-      <c r="H18" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1673,9 +1588,6 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1683,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1691,16 +1603,13 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
-      <c r="H20" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1708,16 +1617,13 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1725,16 +1631,13 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
-      <c r="H22" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1742,16 +1645,13 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1759,16 +1659,13 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
-      <c r="H24" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1776,16 +1673,13 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
-      <c r="H25" s="2" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1799,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1807,9 +1701,6 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1821,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1829,9 +1720,6 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1842,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1860,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1878,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1886,16 +1774,13 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1903,16 +1788,13 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1920,16 +1802,13 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
-      <c r="H33" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1937,14 +1816,11 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1952,16 +1828,13 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1969,16 +1842,13 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1986,16 +1856,13 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -2003,9 +1870,6 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -2013,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -2021,9 +1885,6 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
-      <c r="H39" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -2031,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -2039,9 +1900,6 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
-      <c r="H40" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -2049,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -2057,9 +1915,6 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
-      <c r="H41" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -2067,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -2075,9 +1930,6 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
-      <c r="H42" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -2085,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -2093,9 +1945,6 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
-      <c r="H43" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -2103,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -2111,15 +1960,12 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
-      <c r="H44" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -2127,16 +1973,13 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
-      <c r="H45" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -2144,16 +1987,13 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
-      <c r="H46" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2161,16 +2001,13 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="H47" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2178,14 +2015,11 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-      <c r="H48" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2194,12 +2028,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2207,16 +2041,13 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-      <c r="H50" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2224,16 +2055,13 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-      <c r="H51" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2241,16 +2069,13 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="H52" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2258,16 +2083,13 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-      <c r="H53" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2275,16 +2097,13 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-      <c r="H54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2292,16 +2111,13 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-      <c r="H55" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2309,16 +2125,13 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="H56" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2326,16 +2139,13 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-      <c r="H57" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2343,16 +2153,13 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-      <c r="H58" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2360,16 +2167,13 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-      <c r="H59" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2377,16 +2181,13 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-      <c r="H60" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2394,16 +2195,13 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-      <c r="H61" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2411,16 +2209,13 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-      <c r="H62" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2428,16 +2223,13 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-      <c r="H63" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2445,16 +2237,13 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2462,16 +2251,13 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
-      <c r="H65" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2479,14 +2265,11 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
-      <c r="H66" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2494,9 +2277,6 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
-      <c r="H67" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2527,10 +2307,7 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19">
-        <f>G69-F69</f>
-        <v>0</v>
-      </c>
+      <c r="H69" s="19"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>

<commit_message>
Make changes for trade payable notes
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E26FAA18-BAC9-450D-9471-DBFBF0AEBAA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
   <si>
     <t/>
   </si>
@@ -36,21 +36,36 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>Finance Expenses</t>
+  </si>
+  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
+    <t>Income Tax Expense</t>
+  </si>
+  <si>
     <t>Income tax expense</t>
   </si>
   <si>
+    <t>Administrative Expenses</t>
+  </si>
+  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
+    <t>Other Income</t>
+  </si>
+  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
+    <t>Distribution and Marketing Expenses</t>
+  </si>
+  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -120,30 +135,51 @@
     <t>Accounting fee</t>
   </si>
   <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
     <t>Purchases</t>
   </si>
   <si>
+    <t>Revenue</t>
+  </si>
+  <si>
     <t>Sales</t>
   </si>
   <si>
+    <t>Retained Profits</t>
+  </si>
+  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
+    <t>Current Income Tax Liabilities</t>
+  </si>
+  <si>
     <t>Income tax payable</t>
   </si>
   <si>
+    <t>Amount owing from a Shareholder</t>
+  </si>
+  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
+    <t>GST Payables</t>
+  </si>
+  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -165,9 +201,15 @@
     <t>Prepayments</t>
   </si>
   <si>
+    <t>Deposits</t>
+  </si>
+  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
+    <t>Plant and Equipment</t>
+  </si>
+  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -195,6 +237,9 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
+    <t>Bank Balances</t>
+  </si>
+  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -214,6 +259,15 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>December 2016</t>
+  </si>
+  <si>
+    <t>Trial Balance</t>
+  </si>
+  <si>
+    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -934,7 +988,7 @@
   <dimension ref="A1:AA81"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1345,7 +1399,9 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63"/>
+      <c r="E2" s="63" t="s">
+        <v>79</v>
+      </c>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1355,7 +1411,9 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59"/>
+      <c r="E3" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1365,7 +1423,9 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59"/>
+      <c r="E4" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1375,7 +1435,9 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59"/>
+      <c r="E5" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1385,7 +1447,9 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59"/>
+      <c r="E6" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1395,7 +1459,9 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56"/>
+      <c r="E7" s="56" t="s">
+        <v>78</v>
+      </c>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1405,7 +1471,9 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52"/>
+      <c r="E8" s="52" t="s">
+        <v>77</v>
+      </c>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1426,15 +1494,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1444,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1452,7 +1520,9 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31"/>
+      <c r="H11" s="31" t="s">
+        <v>69</v>
+      </c>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1479,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1487,14 +1557,16 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H12" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1502,14 +1574,16 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H13" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1517,14 +1591,16 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31"/>
+      <c r="H14" s="31" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1538,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1546,13 +1622,16 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
+      <c r="H16" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1560,13 +1639,16 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
+      <c r="H17" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1574,13 +1656,16 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
+      <c r="H18" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1588,6 +1673,9 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
+      <c r="H19" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1595,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1603,13 +1691,16 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
+      <c r="H20" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1617,13 +1708,16 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
+      <c r="H21" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1631,13 +1725,16 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
+      <c r="H22" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1645,13 +1742,16 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
+      <c r="H23" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1659,13 +1759,16 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
+      <c r="H24" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1673,13 +1776,16 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
+      <c r="H25" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1693,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1701,6 +1807,9 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
+      <c r="H27" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1712,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1720,6 +1829,9 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
+      <c r="H28" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1730,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1748,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1766,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1774,13 +1886,16 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1788,13 +1903,16 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1802,13 +1920,16 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
+      <c r="H33" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1816,11 +1937,14 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
+      <c r="H34" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1828,13 +1952,16 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
+      <c r="H35" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1842,13 +1969,16 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1856,13 +1986,16 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -1870,6 +2003,9 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -1877,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -1885,6 +2021,9 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
+      <c r="H39" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -1892,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -1900,6 +2039,9 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
+      <c r="H40" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -1907,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -1915,6 +2057,9 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
+      <c r="H41" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -1922,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -1930,6 +2075,9 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
+      <c r="H42" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -1937,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -1945,6 +2093,9 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
+      <c r="H43" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -1952,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -1960,12 +2111,15 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
+      <c r="H44" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -1973,13 +2127,16 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
+      <c r="H45" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -1987,13 +2144,16 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
+      <c r="H46" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2001,13 +2161,16 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
+      <c r="H47" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2015,11 +2178,14 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2028,12 +2194,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2041,13 +2207,16 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2055,13 +2224,16 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2069,13 +2241,16 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2083,13 +2258,16 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2097,13 +2275,16 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2111,13 +2292,16 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2125,13 +2309,16 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2139,13 +2326,16 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2153,13 +2343,16 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2167,13 +2360,16 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2181,13 +2377,16 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2195,13 +2394,16 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2209,13 +2411,16 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2223,13 +2428,16 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2237,13 +2445,16 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
+      <c r="H64" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2251,13 +2462,16 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
+      <c r="H65" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2265,11 +2479,14 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
+      <c r="H66" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2277,6 +2494,9 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
+      <c r="H67" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2307,7 +2527,10 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19"/>
+      <c r="H69" s="19">
+        <f>G69-F69</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>

<commit_message>
Report now able to be generated with correct output
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F559D3F-FB4B-4925-A6B1-CD2B81203BE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
   <si>
     <t/>
   </si>
@@ -36,36 +36,21 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Finance Expenses</t>
-  </si>
-  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
-    <t>Income Tax Expense</t>
-  </si>
-  <si>
     <t>Income tax expense</t>
   </si>
   <si>
-    <t>Administrative Expenses</t>
-  </si>
-  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
-    <t>Other Income</t>
-  </si>
-  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
-    <t>Distribution and Marketing Expenses</t>
-  </si>
-  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -135,51 +120,30 @@
     <t>Accounting fee</t>
   </si>
   <si>
-    <t>Cost of Sales</t>
-  </si>
-  <si>
     <t>Purchases</t>
   </si>
   <si>
-    <t>Revenue</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>Retained Profits</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
-    <t>Share Capital</t>
-  </si>
-  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
-    <t>Current Income Tax Liabilities</t>
-  </si>
-  <si>
     <t>Income tax payable</t>
   </si>
   <si>
-    <t>Amount owing from a Shareholder</t>
-  </si>
-  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
-    <t>GST Payables</t>
-  </si>
-  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -201,15 +165,9 @@
     <t>Prepayments</t>
   </si>
   <si>
-    <t>Deposits</t>
-  </si>
-  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
-    <t>Plant and Equipment</t>
-  </si>
-  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -237,9 +195,6 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
-    <t>Bank Balances</t>
-  </si>
-  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -259,15 +214,6 @@
   </si>
   <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>December 2016</t>
-  </si>
-  <si>
-    <t>Trial Balance</t>
-  </si>
-  <si>
-    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -987,8 +933,8 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1399,9 +1345,7 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63" t="s">
-        <v>79</v>
-      </c>
+      <c r="E2" s="63"/>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1411,9 +1355,7 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="59"/>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1423,9 +1365,7 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E4" s="59"/>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1435,9 +1375,7 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E5" s="59"/>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1447,9 +1385,7 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="59"/>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1459,9 +1395,7 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56" t="s">
-        <v>78</v>
-      </c>
+      <c r="E7" s="56"/>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1471,9 +1405,7 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52" t="s">
-        <v>77</v>
-      </c>
+      <c r="E8" s="52"/>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1494,15 +1426,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1512,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1520,9 +1452,7 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H11" s="31"/>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1549,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1557,16 +1487,14 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1574,16 +1502,14 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1591,16 +1517,14 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1614,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1622,16 +1546,13 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
-      <c r="H16" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1639,16 +1560,13 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
-      <c r="H17" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1656,16 +1574,13 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
-      <c r="H18" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1673,9 +1588,6 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1683,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1691,16 +1603,13 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
-      <c r="H20" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1708,16 +1617,13 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1725,16 +1631,13 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
-      <c r="H22" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1742,16 +1645,13 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1759,16 +1659,13 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
-      <c r="H24" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1776,16 +1673,13 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
-      <c r="H25" s="2" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1799,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1807,9 +1701,6 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1821,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1829,9 +1720,6 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1842,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1860,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1878,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1886,16 +1774,13 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1903,16 +1788,13 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1920,16 +1802,13 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
-      <c r="H33" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1937,14 +1816,11 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1952,16 +1828,13 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1969,16 +1842,13 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1986,16 +1856,13 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -2003,9 +1870,6 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -2013,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -2021,9 +1885,6 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
-      <c r="H39" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -2031,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -2039,9 +1900,6 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
-      <c r="H40" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -2049,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -2057,9 +1915,6 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
-      <c r="H41" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -2067,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -2075,9 +1930,6 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
-      <c r="H42" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -2085,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -2093,9 +1945,6 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
-      <c r="H43" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -2103,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -2111,15 +1960,12 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
-      <c r="H44" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -2127,16 +1973,13 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
-      <c r="H45" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -2144,16 +1987,13 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
-      <c r="H46" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2161,16 +2001,13 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="H47" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2178,14 +2015,11 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-      <c r="H48" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2194,12 +2028,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2207,16 +2041,13 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-      <c r="H50" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2224,16 +2055,13 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-      <c r="H51" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2241,16 +2069,13 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="H52" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2258,16 +2083,13 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-      <c r="H53" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2275,16 +2097,13 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-      <c r="H54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2292,16 +2111,13 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-      <c r="H55" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2309,16 +2125,13 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="H56" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2326,16 +2139,13 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-      <c r="H57" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2343,16 +2153,13 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-      <c r="H58" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2360,16 +2167,13 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-      <c r="H59" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2377,16 +2181,13 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-      <c r="H60" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2394,16 +2195,13 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-      <c r="H61" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2411,16 +2209,13 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-      <c r="H62" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2428,16 +2223,13 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-      <c r="H63" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2445,16 +2237,13 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2462,16 +2251,13 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
-      <c r="H65" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2479,14 +2265,11 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
-      <c r="H66" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2494,9 +2277,6 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
-      <c r="H67" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2527,10 +2307,7 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19">
-        <f>G69-F69</f>
-        <v>0</v>
-      </c>
+      <c r="H69" s="19"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>

<commit_message>
Changed all of the header in word document
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F559D3F-FB4B-4925-A6B1-CD2B81203BE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
   <si>
     <t/>
   </si>
@@ -36,21 +36,36 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>Finance Expenses</t>
+  </si>
+  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
+    <t>Income Tax Expense</t>
+  </si>
+  <si>
     <t>Income tax expense</t>
   </si>
   <si>
+    <t>Administrative Expenses</t>
+  </si>
+  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
+    <t>Other Income</t>
+  </si>
+  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
+    <t>Distribution and Marketing Expenses</t>
+  </si>
+  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -120,30 +135,51 @@
     <t>Accounting fee</t>
   </si>
   <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
     <t>Purchases</t>
   </si>
   <si>
+    <t>Revenue</t>
+  </si>
+  <si>
     <t>Sales</t>
   </si>
   <si>
+    <t>Retained Profits</t>
+  </si>
+  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
+    <t>Current Income Tax Liabilities</t>
+  </si>
+  <si>
     <t>Income tax payable</t>
   </si>
   <si>
+    <t>Amount owing from a Shareholder</t>
+  </si>
+  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
+    <t>GST Payables</t>
+  </si>
+  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -165,9 +201,15 @@
     <t>Prepayments</t>
   </si>
   <si>
+    <t>Deposits</t>
+  </si>
+  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
+    <t>Plant and Equipment</t>
+  </si>
+  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -195,6 +237,9 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
+    <t>Bank Balances</t>
+  </si>
+  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -214,6 +259,15 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>December 2016</t>
+  </si>
+  <si>
+    <t>Trial Balance</t>
+  </si>
+  <si>
+    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -933,8 +987,8 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H70"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1345,7 +1399,9 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63"/>
+      <c r="E2" s="63" t="s">
+        <v>79</v>
+      </c>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1355,7 +1411,9 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59"/>
+      <c r="E3" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1365,7 +1423,9 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59"/>
+      <c r="E4" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1375,7 +1435,9 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59"/>
+      <c r="E5" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1385,7 +1447,9 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59"/>
+      <c r="E6" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1395,7 +1459,9 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56"/>
+      <c r="E7" s="56" t="s">
+        <v>78</v>
+      </c>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1405,7 +1471,9 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52"/>
+      <c r="E8" s="52" t="s">
+        <v>77</v>
+      </c>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1426,15 +1494,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1444,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1452,7 +1520,9 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31"/>
+      <c r="H11" s="31" t="s">
+        <v>69</v>
+      </c>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1479,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1487,14 +1557,16 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H12" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1502,14 +1574,16 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H13" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1517,14 +1591,16 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31"/>
+      <c r="H14" s="31" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1538,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1546,13 +1622,16 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
+      <c r="H16" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1560,13 +1639,16 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
+      <c r="H17" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1574,13 +1656,16 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
+      <c r="H18" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1588,6 +1673,9 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
+      <c r="H19" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1595,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1603,13 +1691,16 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
+      <c r="H20" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1617,13 +1708,16 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
+      <c r="H21" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1631,13 +1725,16 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
+      <c r="H22" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1645,13 +1742,16 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
+      <c r="H23" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1659,13 +1759,16 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
+      <c r="H24" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1673,13 +1776,16 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
+      <c r="H25" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1693,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1701,6 +1807,9 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
+      <c r="H27" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1712,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1720,6 +1829,9 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
+      <c r="H28" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1730,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1748,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1766,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1774,13 +1886,16 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1788,13 +1903,16 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1802,13 +1920,16 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
+      <c r="H33" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1816,11 +1937,14 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
+      <c r="H34" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1828,13 +1952,16 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
+      <c r="H35" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1842,13 +1969,16 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1856,13 +1986,16 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -1870,6 +2003,9 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -1877,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -1885,6 +2021,9 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
+      <c r="H39" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -1892,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -1900,6 +2039,9 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
+      <c r="H40" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -1907,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -1915,6 +2057,9 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
+      <c r="H41" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -1922,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -1930,6 +2075,9 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
+      <c r="H42" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -1937,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -1945,6 +2093,9 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
+      <c r="H43" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -1952,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -1960,12 +2111,15 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
+      <c r="H44" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -1973,13 +2127,16 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
+      <c r="H45" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -1987,13 +2144,16 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
+      <c r="H46" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2001,13 +2161,16 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
+      <c r="H47" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2015,11 +2178,14 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2028,12 +2194,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2041,13 +2207,16 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2055,13 +2224,16 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2069,13 +2241,16 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2083,13 +2258,16 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2097,13 +2275,16 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2111,13 +2292,16 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2125,13 +2309,16 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2139,13 +2326,16 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2153,13 +2343,16 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2167,13 +2360,16 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2181,13 +2377,16 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2195,13 +2394,16 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2209,13 +2411,16 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2223,13 +2428,16 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2237,13 +2445,16 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
+      <c r="H64" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2251,13 +2462,16 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
+      <c r="H65" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2265,11 +2479,14 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
+      <c r="H66" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2277,6 +2494,9 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
+      <c r="H67" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2307,7 +2527,10 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19"/>
+      <c r="H69" s="19">
+        <f>G69-F69</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>

<commit_message>
Changed all input from notes to smallcaps.
-> update categories not done yet. still in progress
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F559D3F-FB4B-4925-A6B1-CD2B81203BE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
   <si>
     <t/>
   </si>
@@ -36,21 +36,36 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>Finance Expenses</t>
+  </si>
+  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
+    <t>Income Tax Expense</t>
+  </si>
+  <si>
     <t>Income tax expense</t>
   </si>
   <si>
+    <t>Administrative Expenses</t>
+  </si>
+  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
+    <t>Other Income</t>
+  </si>
+  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
+    <t>Distribution and Marketing Expenses</t>
+  </si>
+  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -120,30 +135,51 @@
     <t>Accounting fee</t>
   </si>
   <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
     <t>Purchases</t>
   </si>
   <si>
+    <t>Revenue</t>
+  </si>
+  <si>
     <t>Sales</t>
   </si>
   <si>
+    <t>Retained Profits</t>
+  </si>
+  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
+    <t>Current Income Tax Liabilities</t>
+  </si>
+  <si>
     <t>Income tax payable</t>
   </si>
   <si>
+    <t>Amount owing from a Shareholder</t>
+  </si>
+  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
+    <t>GST Payables</t>
+  </si>
+  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -165,9 +201,15 @@
     <t>Prepayments</t>
   </si>
   <si>
+    <t>Deposits</t>
+  </si>
+  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
+    <t>Plant and Equipment</t>
+  </si>
+  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -195,6 +237,9 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
+    <t>Bank Balances</t>
+  </si>
+  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -214,6 +259,15 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>December 2016</t>
+  </si>
+  <si>
+    <t>Trial Balance</t>
+  </si>
+  <si>
+    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -933,8 +987,8 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H70"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1345,7 +1399,9 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63"/>
+      <c r="E2" s="63" t="s">
+        <v>79</v>
+      </c>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1355,7 +1411,9 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59"/>
+      <c r="E3" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1365,7 +1423,9 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59"/>
+      <c r="E4" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1375,7 +1435,9 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59"/>
+      <c r="E5" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1385,7 +1447,9 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59"/>
+      <c r="E6" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1395,7 +1459,9 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56"/>
+      <c r="E7" s="56" t="s">
+        <v>78</v>
+      </c>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1405,7 +1471,9 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52"/>
+      <c r="E8" s="52" t="s">
+        <v>77</v>
+      </c>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1426,15 +1494,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1444,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1452,7 +1520,9 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31"/>
+      <c r="H11" s="31" t="s">
+        <v>69</v>
+      </c>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1479,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1487,14 +1557,16 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H12" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1502,14 +1574,16 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H13" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1517,14 +1591,16 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31"/>
+      <c r="H14" s="31" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1538,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1546,13 +1622,16 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
+      <c r="H16" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1560,13 +1639,16 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
+      <c r="H17" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1574,13 +1656,16 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
+      <c r="H18" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1588,6 +1673,9 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
+      <c r="H19" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1595,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1603,13 +1691,16 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
+      <c r="H20" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1617,13 +1708,16 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
+      <c r="H21" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1631,13 +1725,16 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
+      <c r="H22" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1645,13 +1742,16 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
+      <c r="H23" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1659,13 +1759,16 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
+      <c r="H24" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1673,13 +1776,16 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
+      <c r="H25" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1693,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1701,6 +1807,9 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
+      <c r="H27" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1712,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1720,6 +1829,9 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
+      <c r="H28" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1730,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1748,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1766,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1774,13 +1886,16 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1788,13 +1903,16 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1802,13 +1920,16 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
+      <c r="H33" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1816,11 +1937,14 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
+      <c r="H34" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1828,13 +1952,16 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
+      <c r="H35" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1842,13 +1969,16 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1856,13 +1986,16 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -1870,6 +2003,9 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -1877,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -1885,6 +2021,9 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
+      <c r="H39" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -1892,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -1900,6 +2039,9 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
+      <c r="H40" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -1907,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -1915,6 +2057,9 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
+      <c r="H41" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -1922,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -1930,6 +2075,9 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
+      <c r="H42" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -1937,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -1945,6 +2093,9 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
+      <c r="H43" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -1952,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -1960,12 +2111,15 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
+      <c r="H44" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -1973,13 +2127,16 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
+      <c r="H45" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -1987,13 +2144,16 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
+      <c r="H46" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2001,13 +2161,16 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
+      <c r="H47" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2015,11 +2178,14 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2028,12 +2194,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2041,13 +2207,16 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2055,13 +2224,16 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2069,13 +2241,16 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2083,13 +2258,16 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2097,13 +2275,16 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2111,13 +2292,16 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2125,13 +2309,16 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2139,13 +2326,16 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2153,13 +2343,16 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2167,13 +2360,16 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2181,13 +2377,16 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2195,13 +2394,16 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2209,13 +2411,16 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2223,13 +2428,16 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2237,13 +2445,16 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
+      <c r="H64" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2251,13 +2462,16 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
+      <c r="H65" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2265,11 +2479,14 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
+      <c r="H66" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2277,6 +2494,9 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
+      <c r="H67" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2307,7 +2527,10 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19"/>
+      <c r="H69" s="19">
+        <f>G69-F69</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>

<commit_message>
Used datalist instead for choosing category (autocomplete)
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F559D3F-FB4B-4925-A6B1-CD2B81203BE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
   <si>
     <t/>
   </si>
@@ -36,36 +36,21 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Finance Expenses</t>
-  </si>
-  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
-    <t>Income Tax Expense</t>
-  </si>
-  <si>
     <t>Income tax expense</t>
   </si>
   <si>
-    <t>Administrative Expenses</t>
-  </si>
-  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
-    <t>Other Income</t>
-  </si>
-  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
-    <t>Distribution and Marketing Expenses</t>
-  </si>
-  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -135,51 +120,30 @@
     <t>Accounting fee</t>
   </si>
   <si>
-    <t>Cost of Sales</t>
-  </si>
-  <si>
     <t>Purchases</t>
   </si>
   <si>
-    <t>Revenue</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>Retained Profits</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
-    <t>Share Capital</t>
-  </si>
-  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
-    <t>Current Income Tax Liabilities</t>
-  </si>
-  <si>
     <t>Income tax payable</t>
   </si>
   <si>
-    <t>Amount owing from a Shareholder</t>
-  </si>
-  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
-    <t>GST Payables</t>
-  </si>
-  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -201,15 +165,9 @@
     <t>Prepayments</t>
   </si>
   <si>
-    <t>Deposits</t>
-  </si>
-  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
-    <t>Plant and Equipment</t>
-  </si>
-  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -237,9 +195,6 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
-    <t>Bank Balances</t>
-  </si>
-  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -259,15 +214,6 @@
   </si>
   <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>December 2016</t>
-  </si>
-  <si>
-    <t>Trial Balance</t>
-  </si>
-  <si>
-    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -987,8 +933,8 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1399,9 +1345,7 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63" t="s">
-        <v>79</v>
-      </c>
+      <c r="E2" s="63"/>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1411,9 +1355,7 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="59"/>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1423,9 +1365,7 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E4" s="59"/>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1435,9 +1375,7 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E5" s="59"/>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1447,9 +1385,7 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="59"/>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1459,9 +1395,7 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56" t="s">
-        <v>78</v>
-      </c>
+      <c r="E7" s="56"/>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1471,9 +1405,7 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52" t="s">
-        <v>77</v>
-      </c>
+      <c r="E8" s="52"/>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1494,15 +1426,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1512,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1520,9 +1452,7 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H11" s="31"/>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1549,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1557,16 +1487,14 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1574,16 +1502,14 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1591,16 +1517,14 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1614,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1622,16 +1546,13 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
-      <c r="H16" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1639,16 +1560,13 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
-      <c r="H17" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1656,16 +1574,13 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
-      <c r="H18" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1673,9 +1588,6 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1683,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1691,16 +1603,13 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
-      <c r="H20" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1708,16 +1617,13 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1725,16 +1631,13 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
-      <c r="H22" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1742,16 +1645,13 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1759,16 +1659,13 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
-      <c r="H24" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1776,16 +1673,13 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
-      <c r="H25" s="2" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1799,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1807,9 +1701,6 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1821,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1829,9 +1720,6 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1842,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1860,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1878,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1886,16 +1774,13 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1903,16 +1788,13 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1920,16 +1802,13 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
-      <c r="H33" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1937,14 +1816,11 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1952,16 +1828,13 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1969,16 +1842,13 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1986,16 +1856,13 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -2003,9 +1870,6 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -2013,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -2021,9 +1885,6 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
-      <c r="H39" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -2031,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -2039,9 +1900,6 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
-      <c r="H40" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -2049,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -2057,9 +1915,6 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
-      <c r="H41" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -2067,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -2075,9 +1930,6 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
-      <c r="H42" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -2085,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -2093,9 +1945,6 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
-      <c r="H43" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -2103,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -2111,15 +1960,12 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
-      <c r="H44" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -2127,16 +1973,13 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
-      <c r="H45" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -2144,16 +1987,13 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
-      <c r="H46" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2161,16 +2001,13 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="H47" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2178,14 +2015,11 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-      <c r="H48" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2194,12 +2028,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2207,16 +2041,13 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-      <c r="H50" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2224,16 +2055,13 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-      <c r="H51" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2241,16 +2069,13 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="H52" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2258,16 +2083,13 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-      <c r="H53" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2275,16 +2097,13 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-      <c r="H54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2292,16 +2111,13 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-      <c r="H55" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2309,16 +2125,13 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="H56" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2326,16 +2139,13 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-      <c r="H57" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2343,16 +2153,13 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-      <c r="H58" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2360,16 +2167,13 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-      <c r="H59" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2377,16 +2181,13 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-      <c r="H60" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2394,16 +2195,13 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-      <c r="H61" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2411,16 +2209,13 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-      <c r="H62" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2428,16 +2223,13 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-      <c r="H63" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2445,16 +2237,13 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2462,16 +2251,13 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
-      <c r="H65" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2479,14 +2265,11 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
-      <c r="H66" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2494,9 +2277,6 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
-      <c r="H67" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2527,10 +2307,7 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19">
-        <f>G69-F69</f>
-        <v>0</v>
-      </c>
+      <c r="H69" s="19"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>

<commit_message>
update categories, insert empty field complete
-> left checking of newly changes
-> and new category
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F559D3F-FB4B-4925-A6B1-CD2B81203BE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
   <si>
     <t/>
   </si>
@@ -36,21 +36,36 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>Finance Expenses</t>
+  </si>
+  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
+    <t>Income Tax Expense</t>
+  </si>
+  <si>
     <t>Income tax expense</t>
   </si>
   <si>
+    <t>Administrative Expenses</t>
+  </si>
+  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
+    <t>Other Income</t>
+  </si>
+  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
+    <t>Distribution and Marketing Expenses</t>
+  </si>
+  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -120,30 +135,51 @@
     <t>Accounting fee</t>
   </si>
   <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
     <t>Purchases</t>
   </si>
   <si>
+    <t>Revenue</t>
+  </si>
+  <si>
     <t>Sales</t>
   </si>
   <si>
+    <t>Retained Profits</t>
+  </si>
+  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
+    <t>Current Income Tax Liabilities</t>
+  </si>
+  <si>
     <t>Income tax payable</t>
   </si>
   <si>
+    <t>Amount owing from a Shareholder</t>
+  </si>
+  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
+    <t>GST Payables</t>
+  </si>
+  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -165,9 +201,15 @@
     <t>Prepayments</t>
   </si>
   <si>
+    <t>Deposits</t>
+  </si>
+  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
+    <t>Plant and Equipment</t>
+  </si>
+  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -195,6 +237,9 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
+    <t>Bank Balances</t>
+  </si>
+  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -214,6 +259,15 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>December 2016</t>
+  </si>
+  <si>
+    <t>Trial Balance</t>
+  </si>
+  <si>
+    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -933,8 +987,8 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H70"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1345,7 +1399,9 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63"/>
+      <c r="E2" s="63" t="s">
+        <v>79</v>
+      </c>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1355,7 +1411,9 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59"/>
+      <c r="E3" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1365,7 +1423,9 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59"/>
+      <c r="E4" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1375,7 +1435,9 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59"/>
+      <c r="E5" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1385,7 +1447,9 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59"/>
+      <c r="E6" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1395,7 +1459,9 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56"/>
+      <c r="E7" s="56" t="s">
+        <v>78</v>
+      </c>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1405,7 +1471,9 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52"/>
+      <c r="E8" s="52" t="s">
+        <v>77</v>
+      </c>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1426,15 +1494,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1444,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1452,7 +1520,9 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31"/>
+      <c r="H11" s="31" t="s">
+        <v>69</v>
+      </c>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1479,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1487,14 +1557,16 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H12" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1502,14 +1574,16 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H13" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1517,14 +1591,16 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31"/>
+      <c r="H14" s="31" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1538,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1546,13 +1622,16 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
+      <c r="H16" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1560,13 +1639,16 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
+      <c r="H17" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1574,13 +1656,16 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
+      <c r="H18" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1588,6 +1673,9 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
+      <c r="H19" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1595,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1603,13 +1691,16 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
+      <c r="H20" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1617,13 +1708,16 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
+      <c r="H21" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1631,13 +1725,16 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
+      <c r="H22" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1645,13 +1742,16 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
+      <c r="H23" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1659,13 +1759,16 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
+      <c r="H24" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1673,13 +1776,16 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
+      <c r="H25" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1693,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1701,6 +1807,9 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
+      <c r="H27" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1712,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1720,6 +1829,9 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
+      <c r="H28" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1730,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1748,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1766,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1774,13 +1886,16 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1788,13 +1903,16 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1802,13 +1920,16 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
+      <c r="H33" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1816,11 +1937,14 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
+      <c r="H34" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1828,13 +1952,16 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
+      <c r="H35" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1842,13 +1969,16 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1856,13 +1986,16 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -1870,6 +2003,9 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -1877,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -1885,6 +2021,9 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
+      <c r="H39" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -1892,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -1900,6 +2039,9 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
+      <c r="H40" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -1907,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -1915,6 +2057,9 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
+      <c r="H41" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -1922,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -1930,6 +2075,9 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
+      <c r="H42" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -1937,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -1945,6 +2093,9 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
+      <c r="H43" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -1952,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -1960,12 +2111,15 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
+      <c r="H44" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -1973,13 +2127,16 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
+      <c r="H45" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -1987,13 +2144,16 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
+      <c r="H46" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2001,13 +2161,16 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
+      <c r="H47" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2015,11 +2178,14 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2028,12 +2194,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2041,13 +2207,16 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2055,13 +2224,16 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2069,13 +2241,16 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2083,13 +2258,16 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2097,13 +2275,16 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2111,13 +2292,16 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2125,13 +2309,16 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2139,13 +2326,16 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2153,13 +2343,16 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2167,13 +2360,16 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2181,13 +2377,16 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2195,13 +2394,16 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2209,13 +2411,16 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2223,13 +2428,16 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2237,13 +2445,16 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
+      <c r="H64" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2251,13 +2462,16 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
+      <c r="H65" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2265,11 +2479,14 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
+      <c r="H66" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2277,6 +2494,9 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
+      <c r="H67" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2307,7 +2527,10 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19"/>
+      <c r="H69" s="19">
+        <f>G69-F69</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>

<commit_message>
Fixed warning in client admin page
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E26FAA18-BAC9-450D-9471-DBFBF0AEBAA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
   <si>
     <t/>
   </si>
@@ -36,36 +36,21 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Finance Expenses</t>
-  </si>
-  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
-    <t>Income Tax Expense</t>
-  </si>
-  <si>
     <t>Income tax expense</t>
   </si>
   <si>
-    <t>Administrative Expenses</t>
-  </si>
-  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
-    <t>Other Income</t>
-  </si>
-  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
-    <t>Distribution and Marketing Expenses</t>
-  </si>
-  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -135,51 +120,30 @@
     <t>Accounting fee</t>
   </si>
   <si>
-    <t>Cost of Sales</t>
-  </si>
-  <si>
     <t>Purchases</t>
   </si>
   <si>
-    <t>Revenue</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>Retained Profits</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
-    <t>Share Capital</t>
-  </si>
-  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
-    <t>Current Income Tax Liabilities</t>
-  </si>
-  <si>
     <t>Income tax payable</t>
   </si>
   <si>
-    <t>Amount owing from a Shareholder</t>
-  </si>
-  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
-    <t>GST Payables</t>
-  </si>
-  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -201,15 +165,9 @@
     <t>Prepayments</t>
   </si>
   <si>
-    <t>Deposits</t>
-  </si>
-  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
-    <t>Plant and Equipment</t>
-  </si>
-  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -237,9 +195,6 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
-    <t>Bank Balances</t>
-  </si>
-  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -259,15 +214,6 @@
   </si>
   <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>December 2016</t>
-  </si>
-  <si>
-    <t>Trial Balance</t>
-  </si>
-  <si>
-    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -988,7 +934,7 @@
   <dimension ref="A1:AA81"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1399,9 +1345,7 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63" t="s">
-        <v>79</v>
-      </c>
+      <c r="E2" s="63"/>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1411,9 +1355,7 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="59"/>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1423,9 +1365,7 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E4" s="59"/>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1435,9 +1375,7 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E5" s="59"/>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1447,9 +1385,7 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="59"/>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1459,9 +1395,7 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56" t="s">
-        <v>78</v>
-      </c>
+      <c r="E7" s="56"/>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1471,9 +1405,7 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52" t="s">
-        <v>77</v>
-      </c>
+      <c r="E8" s="52"/>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1494,15 +1426,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1512,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1520,9 +1452,7 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H11" s="31"/>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1549,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1557,16 +1487,14 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1574,16 +1502,14 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1591,16 +1517,14 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1614,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1622,16 +1546,13 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
-      <c r="H16" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1639,16 +1560,13 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
-      <c r="H17" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1656,16 +1574,13 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
-      <c r="H18" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1673,9 +1588,6 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1683,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1691,16 +1603,13 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
-      <c r="H20" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1708,16 +1617,13 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1725,16 +1631,13 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
-      <c r="H22" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1742,16 +1645,13 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1759,16 +1659,13 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
-      <c r="H24" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1776,16 +1673,13 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
-      <c r="H25" s="2" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1799,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1807,9 +1701,6 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1821,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1829,9 +1720,6 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1842,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1860,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1878,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1886,16 +1774,13 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1903,16 +1788,13 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1920,16 +1802,13 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
-      <c r="H33" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1937,14 +1816,11 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1952,16 +1828,13 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1969,16 +1842,13 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1986,16 +1856,13 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -2003,9 +1870,6 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -2013,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -2021,9 +1885,6 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
-      <c r="H39" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -2031,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -2039,9 +1900,6 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
-      <c r="H40" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -2049,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -2057,9 +1915,6 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
-      <c r="H41" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -2067,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -2075,9 +1930,6 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
-      <c r="H42" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -2085,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -2093,9 +1945,6 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
-      <c r="H43" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -2103,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -2111,15 +1960,12 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
-      <c r="H44" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -2127,16 +1973,13 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
-      <c r="H45" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -2144,16 +1987,13 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
-      <c r="H46" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2161,16 +2001,13 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="H47" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2178,14 +2015,11 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-      <c r="H48" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2194,12 +2028,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2207,16 +2041,13 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-      <c r="H50" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2224,16 +2055,13 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-      <c r="H51" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2241,16 +2069,13 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="H52" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2258,16 +2083,13 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-      <c r="H53" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2275,16 +2097,13 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-      <c r="H54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2292,16 +2111,13 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-      <c r="H55" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2309,16 +2125,13 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="H56" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2326,16 +2139,13 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-      <c r="H57" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2343,16 +2153,13 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-      <c r="H58" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2360,16 +2167,13 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-      <c r="H59" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2377,16 +2181,13 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-      <c r="H60" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2394,16 +2195,13 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-      <c r="H61" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2411,16 +2209,13 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-      <c r="H62" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2428,16 +2223,13 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-      <c r="H63" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2445,16 +2237,13 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2462,16 +2251,13 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
-      <c r="H65" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2479,14 +2265,11 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
-      <c r="H66" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2494,9 +2277,6 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
-      <c r="H67" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2527,10 +2307,7 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19">
-        <f>G69-F69</f>
-        <v>0</v>
-      </c>
+      <c r="H69" s="19"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>

<commit_message>
Changed the default values for account category
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F559D3F-FB4B-4925-A6B1-CD2B81203BE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
   <si>
     <t/>
   </si>
@@ -36,36 +36,21 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Finance Expenses</t>
-  </si>
-  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
-    <t>Income Tax Expense</t>
-  </si>
-  <si>
     <t>Income tax expense</t>
   </si>
   <si>
-    <t>Administrative Expenses</t>
-  </si>
-  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
-    <t>Other Income</t>
-  </si>
-  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
-    <t>Distribution and Marketing Expenses</t>
-  </si>
-  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -135,51 +120,30 @@
     <t>Accounting fee</t>
   </si>
   <si>
-    <t>Cost of Sales</t>
-  </si>
-  <si>
     <t>Purchases</t>
   </si>
   <si>
-    <t>Revenue</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
-    <t>Retained Profits</t>
-  </si>
-  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
-    <t>Share Capital</t>
-  </si>
-  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
-    <t>Current Income Tax Liabilities</t>
-  </si>
-  <si>
     <t>Income tax payable</t>
   </si>
   <si>
-    <t>Amount owing from a Shareholder</t>
-  </si>
-  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
-    <t>GST Payables</t>
-  </si>
-  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -201,15 +165,9 @@
     <t>Prepayments</t>
   </si>
   <si>
-    <t>Deposits</t>
-  </si>
-  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
-    <t>Plant and Equipment</t>
-  </si>
-  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -237,9 +195,6 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
-    <t>Bank Balances</t>
-  </si>
-  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -259,15 +214,6 @@
   </si>
   <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>December 2016</t>
-  </si>
-  <si>
-    <t>Trial Balance</t>
-  </si>
-  <si>
-    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -987,8 +933,8 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1399,9 +1345,7 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63" t="s">
-        <v>79</v>
-      </c>
+      <c r="E2" s="63"/>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1411,9 +1355,7 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="59"/>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1423,9 +1365,7 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E4" s="59"/>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1435,9 +1375,7 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E5" s="59"/>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1447,9 +1385,7 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="59"/>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1459,9 +1395,7 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56" t="s">
-        <v>78</v>
-      </c>
+      <c r="E7" s="56"/>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1471,9 +1405,7 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52" t="s">
-        <v>77</v>
-      </c>
+      <c r="E8" s="52"/>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1494,15 +1426,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1512,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1520,9 +1452,7 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H11" s="31"/>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1549,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1557,16 +1487,14 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1574,16 +1502,14 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1591,16 +1517,14 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31" t="s">
-        <v>69</v>
-      </c>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1614,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1622,16 +1546,13 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
-      <c r="H16" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1639,16 +1560,13 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
-      <c r="H17" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1656,16 +1574,13 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
-      <c r="H18" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1673,9 +1588,6 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1683,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1691,16 +1603,13 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
-      <c r="H20" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1708,16 +1617,13 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1725,16 +1631,13 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
-      <c r="H22" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1742,16 +1645,13 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1759,16 +1659,13 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
-      <c r="H24" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1776,16 +1673,13 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
-      <c r="H25" s="2" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1799,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1807,9 +1701,6 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1821,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1829,9 +1720,6 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1842,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1860,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1878,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1886,16 +1774,13 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1903,16 +1788,13 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1920,16 +1802,13 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
-      <c r="H33" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1937,14 +1816,11 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1952,16 +1828,13 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1969,16 +1842,13 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1986,16 +1856,13 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -2003,9 +1870,6 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -2013,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -2021,9 +1885,6 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
-      <c r="H39" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -2031,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -2039,9 +1900,6 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
-      <c r="H40" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -2049,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -2057,9 +1915,6 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
-      <c r="H41" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -2067,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -2075,9 +1930,6 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
-      <c r="H42" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -2085,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -2093,9 +1945,6 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
-      <c r="H43" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -2103,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -2111,15 +1960,12 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
-      <c r="H44" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -2127,16 +1973,13 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
-      <c r="H45" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -2144,16 +1987,13 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
-      <c r="H46" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2161,16 +2001,13 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="H47" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2178,14 +2015,11 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-      <c r="H48" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2194,12 +2028,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2207,16 +2041,13 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-      <c r="H50" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2224,16 +2055,13 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-      <c r="H51" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2241,16 +2069,13 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="H52" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2258,16 +2083,13 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-      <c r="H53" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2275,16 +2097,13 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-      <c r="H54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2292,16 +2111,13 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-      <c r="H55" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2309,16 +2125,13 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="H56" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2326,16 +2139,13 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-      <c r="H57" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2343,16 +2153,13 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-      <c r="H58" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2360,16 +2167,13 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-      <c r="H59" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2377,16 +2181,13 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-      <c r="H60" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2394,16 +2195,13 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-      <c r="H61" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2411,16 +2209,13 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-      <c r="H62" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2428,16 +2223,13 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-      <c r="H63" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2445,16 +2237,13 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2462,16 +2251,13 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
-      <c r="H65" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2479,14 +2265,11 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
-      <c r="H66" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2494,9 +2277,6 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
-      <c r="H67" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2527,10 +2307,7 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19">
-        <f>G69-F69</f>
-        <v>0</v>
-      </c>
+      <c r="H69" s="19"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>

<commit_message>
Fixed dropdown in update categories pages not showing list for empty original value
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F559D3F-FB4B-4925-A6B1-CD2B81203BE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E26FAA18-BAC9-450D-9471-DBFBF0AEBAA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -933,8 +933,8 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H70"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Edited Temp Real notes section
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance) one page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\weeko\Downloads\Documents\SIT\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E26FAA18-BAC9-450D-9471-DBFBF0AEBAA7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4DF25F07-99A1-4DD2-B45F-4CCB43813680}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
   <si>
     <t/>
   </si>
@@ -36,21 +36,36 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>Finance Expenses</t>
+  </si>
+  <si>
     <t>Interest on bank borrowings</t>
   </si>
   <si>
+    <t>Income Tax Expense</t>
+  </si>
+  <si>
     <t>Income tax expense</t>
   </si>
   <si>
+    <t>Administrative Expenses</t>
+  </si>
+  <si>
     <t>Unrealised exch - Non trade</t>
   </si>
   <si>
+    <t>Other Income</t>
+  </si>
+  <si>
     <t>Unrealised exchange difference</t>
   </si>
   <si>
     <t>Exchange difference</t>
   </si>
   <si>
+    <t>Distribution and Marketing Expenses</t>
+  </si>
+  <si>
     <t>Travelling</t>
   </si>
   <si>
@@ -120,30 +135,51 @@
     <t>Accounting fee</t>
   </si>
   <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
     <t>Purchases</t>
   </si>
   <si>
+    <t>Revenue</t>
+  </si>
+  <si>
     <t>Sales</t>
   </si>
   <si>
+    <t>Retained Profits</t>
+  </si>
+  <si>
     <t>Retained Earnings</t>
   </si>
   <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
     <t>Paid Up Capital</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
+    <t>Current Income Tax Liabilities</t>
+  </si>
+  <si>
     <t>Income tax payable</t>
   </si>
   <si>
+    <t>Amount owing from a Shareholder</t>
+  </si>
+  <si>
     <t>Amount owing to/(from) SH</t>
   </si>
   <si>
     <t>Accruals</t>
   </si>
   <si>
+    <t>GST Payables</t>
+  </si>
+  <si>
     <t>GST control</t>
   </si>
   <si>
@@ -165,9 +201,15 @@
     <t>Prepayments</t>
   </si>
   <si>
+    <t>Deposits</t>
+  </si>
+  <si>
     <t>Deposits Paid</t>
   </si>
   <si>
+    <t>Plant and Equipment</t>
+  </si>
+  <si>
     <t>Computer and servers - acc dep</t>
   </si>
   <si>
@@ -195,6 +237,9 @@
     <t>Trade Receivables - USD</t>
   </si>
   <si>
+    <t>Bank Balances</t>
+  </si>
+  <si>
     <t>OCBC - USD Exchange</t>
   </si>
   <si>
@@ -214,6 +259,15 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>December 2016</t>
+  </si>
+  <si>
+    <t>Trial Balance</t>
+  </si>
+  <si>
+    <t>VSIG Pte. Ltd.</t>
   </si>
 </sst>
 </file>
@@ -934,7 +988,7 @@
   <dimension ref="A1:AA81"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1345,7 +1399,9 @@
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="63"/>
+      <c r="E2" s="63" t="s">
+        <v>79</v>
+      </c>
       <c r="F2" s="62"/>
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
@@ -1355,7 +1411,9 @@
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="53"/>
-      <c r="E3" s="59"/>
+      <c r="E3" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="58"/>
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
@@ -1365,7 +1423,9 @@
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="59"/>
+      <c r="E4" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F4" s="58"/>
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
@@ -1375,7 +1435,9 @@
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="59"/>
+      <c r="E5" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" s="58"/>
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
@@ -1385,7 +1447,9 @@
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="53"/>
-      <c r="E6" s="59"/>
+      <c r="E6" s="59" t="s">
+        <v>0</v>
+      </c>
       <c r="F6" s="58"/>
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
@@ -1395,7 +1459,9 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" s="53"/>
-      <c r="E7" s="56"/>
+      <c r="E7" s="56" t="s">
+        <v>78</v>
+      </c>
       <c r="F7" s="51"/>
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
@@ -1405,7 +1471,9 @@
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
       <c r="D8" s="53"/>
-      <c r="E8" s="52"/>
+      <c r="E8" s="52" t="s">
+        <v>77</v>
+      </c>
       <c r="F8" s="51"/>
       <c r="G8" s="47"/>
       <c r="H8" s="46"/>
@@ -1426,15 +1494,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="41" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="H10" s="39"/>
     </row>
@@ -1444,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1452,7 +1520,9 @@
         <v>388470.78</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="31"/>
+      <c r="H11" s="31" t="s">
+        <v>69</v>
+      </c>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
@@ -1479,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
@@ -1487,14 +1557,16 @@
         <v>14.71</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="33"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H12" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -1502,14 +1574,16 @@
         <v>978749.17</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H13" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1517,14 +1591,16 @@
         <v>436815.75</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="H14" s="31"/>
+      <c r="H14" s="31" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1538,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1546,13 +1622,16 @@
         <v>203352.09</v>
       </c>
       <c r="G16" s="22"/>
+      <c r="H16" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1560,13 +1639,16 @@
         <v>90756.04</v>
       </c>
       <c r="G17" s="22"/>
+      <c r="H17" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1574,13 +1656,16 @@
         <v>2808</v>
       </c>
       <c r="G18" s="22"/>
+      <c r="H18" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1588,6 +1673,9 @@
       <c r="G19" s="26">
         <v>1392</v>
       </c>
+      <c r="H19" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="J19" s="27"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
@@ -1595,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1603,13 +1691,16 @@
         <v>33024.29</v>
       </c>
       <c r="G20" s="22"/>
+      <c r="H20" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1617,13 +1708,16 @@
       <c r="G21" s="26">
         <v>7607.43</v>
       </c>
+      <c r="H21" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -1631,13 +1725,16 @@
         <v>6233</v>
       </c>
       <c r="G22" s="22"/>
+      <c r="H22" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1645,13 +1742,16 @@
       <c r="G23" s="26">
         <v>2077.66</v>
       </c>
+      <c r="H23" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1659,13 +1759,16 @@
         <v>18458.96</v>
       </c>
       <c r="G24" s="22"/>
+      <c r="H24" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1673,13 +1776,16 @@
         <v>300</v>
       </c>
       <c r="G25" s="22"/>
+      <c r="H25" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -1693,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1701,6 +1807,9 @@
       <c r="G27" s="26">
         <v>166951</v>
       </c>
+      <c r="H27" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="27">
         <f>K29-K28</f>
@@ -1712,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1720,6 +1829,9 @@
       <c r="G28" s="26">
         <v>74531</v>
       </c>
+      <c r="H28" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J28" s="27"/>
       <c r="K28" s="27">
         <v>74531</v>
@@ -1730,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -1748,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -1766,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -1774,13 +1886,16 @@
       <c r="G31" s="26">
         <v>21718.21</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1788,13 +1903,16 @@
       <c r="G32" s="26">
         <v>4650</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -1802,13 +1920,16 @@
         <v>453411.99</v>
       </c>
       <c r="G33" s="22"/>
+      <c r="H33" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -1816,11 +1937,14 @@
       <c r="G34" s="26">
         <v>135951.23000000001</v>
       </c>
+      <c r="H34" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="17" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -1828,13 +1952,16 @@
       <c r="G35" s="26">
         <v>76413.350000000006</v>
       </c>
+      <c r="H35" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -1842,13 +1969,16 @@
       <c r="G36" s="26">
         <v>500000</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -1856,13 +1986,16 @@
       <c r="G37" s="26">
         <v>1004167.9</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -1870,6 +2003,9 @@
       <c r="G38" s="26">
         <v>2168613.73</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="K38" s="27"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -1877,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -1885,6 +2021,9 @@
         <v>1338881.93</v>
       </c>
       <c r="G39" s="22"/>
+      <c r="H39" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K39" s="28"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -1892,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -1900,6 +2039,9 @@
         <v>5100</v>
       </c>
       <c r="G40" s="22"/>
+      <c r="H40" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K40" s="27"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -1907,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -1915,6 +2057,9 @@
         <v>722.31</v>
       </c>
       <c r="G41" s="22"/>
+      <c r="H41" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
@@ -1922,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
@@ -1930,6 +2075,9 @@
         <v>472.23</v>
       </c>
       <c r="G42" s="22"/>
+      <c r="H42" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K42" s="27"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -1937,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
@@ -1945,6 +2093,9 @@
         <v>900</v>
       </c>
       <c r="G43" s="22"/>
+      <c r="H43" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
@@ -1952,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -1960,12 +2111,15 @@
         <v>3013.66</v>
       </c>
       <c r="G44" s="22"/>
+      <c r="H44" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="K44" s="27"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="18"/>
       <c r="C45" s="17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
@@ -1973,13 +2127,16 @@
         <v>36000</v>
       </c>
       <c r="G45" s="22"/>
+      <c r="H45" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -1987,13 +2144,16 @@
         <v>500.49</v>
       </c>
       <c r="G46" s="22"/>
+      <c r="H46" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
@@ -2001,13 +2161,16 @@
         <v>87.52</v>
       </c>
       <c r="G47" s="22"/>
+      <c r="H47" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
@@ -2015,11 +2178,14 @@
         <v>10.28</v>
       </c>
       <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="18"/>
       <c r="C49" s="17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
@@ -2028,12 +2194,12 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -2041,13 +2207,16 @@
         <v>3450</v>
       </c>
       <c r="G50" s="22"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -2055,13 +2224,16 @@
         <v>3.5</v>
       </c>
       <c r="G51" s="22"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -2069,13 +2241,16 @@
         <v>600</v>
       </c>
       <c r="G52" s="22"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2083,13 +2258,16 @@
         <v>258.99</v>
       </c>
       <c r="G53" s="22"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -2097,13 +2275,16 @@
         <v>3600</v>
       </c>
       <c r="G54" s="22"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
@@ -2111,13 +2292,16 @@
         <v>997.5</v>
       </c>
       <c r="G55" s="22"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
@@ -2125,13 +2309,16 @@
         <v>156483.87</v>
       </c>
       <c r="G56" s="22"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
@@ -2139,13 +2326,16 @@
         <v>180</v>
       </c>
       <c r="G57" s="22"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
@@ -2153,13 +2343,16 @@
         <v>437.5</v>
       </c>
       <c r="G58" s="22"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
@@ -2167,13 +2360,16 @@
         <v>243.89</v>
       </c>
       <c r="G59" s="22"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
@@ -2181,13 +2377,16 @@
         <v>154.56</v>
       </c>
       <c r="G60" s="22"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -2195,13 +2394,16 @@
         <v>1200</v>
       </c>
       <c r="G61" s="22"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
@@ -2209,13 +2411,16 @@
         <v>650.77</v>
       </c>
       <c r="G62" s="22"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
@@ -2223,13 +2428,16 @@
         <v>13642.77</v>
       </c>
       <c r="G63" s="22"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
@@ -2237,13 +2445,16 @@
       <c r="G64" s="26">
         <v>62733.24</v>
       </c>
+      <c r="H64" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
@@ -2251,13 +2462,16 @@
         <v>9666.3799999999992</v>
       </c>
       <c r="G65" s="22"/>
+      <c r="H65" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
@@ -2265,11 +2479,14 @@
         <v>36462.82</v>
       </c>
       <c r="G66" s="22"/>
+      <c r="H66" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="18"/>
       <c r="C67" s="17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2277,6 +2494,9 @@
         <v>191</v>
       </c>
       <c r="G67" s="22"/>
+      <c r="H67" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="18" t="s">
@@ -2307,7 +2527,10 @@
         <f>SUM(G11:G67)</f>
         <v>4226806.75</v>
       </c>
-      <c r="H69" s="19"/>
+      <c r="H69" s="19">
+        <f>G69-F69</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">

</xml_diff>